<commit_message>
editing datatable prep script
</commit_message>
<xml_diff>
--- a/eDNA/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
+++ b/eDNA/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
@@ -1012,7 +1012,7 @@
         <v>228</v>
       </c>
       <c r="G9">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9">
         <v>108</v>
@@ -1083,7 +1083,7 @@
         <v>228</v>
       </c>
       <c r="G10">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10">
         <v>107</v>
@@ -1154,7 +1154,7 @@
         <v>228</v>
       </c>
       <c r="G11">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11">
         <v>107</v>
@@ -1225,7 +1225,7 @@
         <v>228</v>
       </c>
       <c r="G12">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12">
         <v>107</v>

</xml_diff>

<commit_message>
datatable prep 02.Rmd and taxonomic assignment
</commit_message>
<xml_diff>
--- a/eDNA/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
+++ b/eDNA/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -488,6 +488,11 @@
           <t>species</t>
         </is>
       </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Choice</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
editing the df prep rmd but still need to produce md file
</commit_message>
<xml_diff>
--- a/eDNA/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
+++ b/eDNA/example_output/Taxonomic_assignments/Choice_required_GMGI_multiplehits.xlsx
@@ -511,10 +511,8 @@
       <c r="D2">
         <v>98.131</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E2">
+        <v>100</v>
       </c>
       <c r="F2">
         <v>34</v>
@@ -582,10 +580,8 @@
       <c r="D3">
         <v>98.131</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E3">
+        <v>100</v>
       </c>
       <c r="F3">
         <v>34</v>
@@ -653,10 +649,8 @@
       <c r="D4">
         <v>98.131</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E4">
+        <v>100</v>
       </c>
       <c r="F4">
         <v>34</v>
@@ -724,10 +718,8 @@
       <c r="D5">
         <v>98.131</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E5">
+        <v>100</v>
       </c>
       <c r="F5">
         <v>34</v>
@@ -795,10 +787,8 @@
       <c r="D6">
         <v>98.131</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E6">
+        <v>100</v>
       </c>
       <c r="F6">
         <v>34</v>
@@ -866,10 +856,8 @@
       <c r="D7">
         <v>100</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E7">
+        <v>100</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -937,10 +925,8 @@
       <c r="D8">
         <v>100</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E8">
+        <v>100</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1008,11 +994,6 @@
       <c r="D9">
         <v>100</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ref2</t>
-        </is>
-      </c>
       <c r="F9">
         <v>228</v>
       </c>
@@ -1045,21 +1026,6 @@
       </c>
       <c r="P9">
         <v>200</v>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Great black backed gull and other gulls</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Larus sp</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>Bird</t>
-        </is>
       </c>
     </row>
     <row r="10">
@@ -1079,11 +1045,6 @@
       <c r="D10">
         <v>100</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>ref1</t>
-        </is>
-      </c>
       <c r="F10">
         <v>228</v>
       </c>
@@ -1116,21 +1077,6 @@
       </c>
       <c r="P10">
         <v>198</v>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Great black backed gull and other gulls</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Larus sp</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>Bird</t>
-        </is>
       </c>
     </row>
     <row r="11">
@@ -1150,10 +1096,8 @@
       <c r="D11">
         <v>99.065</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E11">
+        <v>100</v>
       </c>
       <c r="F11">
         <v>228</v>
@@ -1221,10 +1165,8 @@
       <c r="D12">
         <v>99.065</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E12">
+        <v>100</v>
       </c>
       <c r="F12">
         <v>228</v>

</xml_diff>